<commit_message>
update: schadefactor gras (engelse definitie)
git-svn-id: https://repos.deltares.nl/repos/WettelijkToetsInstrumentarium/trunk@1409 5a3db67b-de53-47b5-99c8-a1c30a6650e2

Former-commit-id: 01dda8e68aaf61df8255827bd2aee39923b9617c
</commit_message>
<xml_diff>
--- a/doc/conventions/Complete WTI parameterlijst Aquo.xlsx
+++ b/doc/conventions/Complete WTI parameterlijst Aquo.xlsx
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9519" uniqueCount="2271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9519" uniqueCount="2272">
   <si>
     <t>ID</t>
   </si>
@@ -11382,6 +11382,9 @@
   </si>
   <si>
     <t>Toeslag volume</t>
+  </si>
+  <si>
+    <t>Damage safety factor</t>
   </si>
 </sst>
 </file>
@@ -16134,6 +16137,25 @@
     <xf numFmtId="0" fontId="17" fillId="12" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="88" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="88" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -16149,25 +16171,6 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="88" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="88" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="61">
     <cellStyle name="Neutraal 2" xfId="3"/>
@@ -20572,7 +20575,7 @@
       <c r="J101" s="992" t="s">
         <v>15</v>
       </c>
-      <c r="K101" s="1312" t="s">
+      <c r="K101" s="1307" t="s">
         <v>172</v>
       </c>
       <c r="L101" s="111"/>
@@ -20606,10 +20609,10 @@
         <v>1125</v>
       </c>
       <c r="I102" s="111"/>
-      <c r="J102" s="1312" t="s">
+      <c r="J102" s="1307" t="s">
         <v>1556</v>
       </c>
-      <c r="K102" s="1314" t="s">
+      <c r="K102" s="1309" t="s">
         <v>18</v>
       </c>
       <c r="L102" s="111"/>
@@ -20641,10 +20644,10 @@
         <v>14</v>
       </c>
       <c r="I103" s="111"/>
-      <c r="J103" s="1313" t="s">
-        <v>18</v>
-      </c>
-      <c r="K103" s="1314" t="s">
+      <c r="J103" s="1308" t="s">
+        <v>18</v>
+      </c>
+      <c r="K103" s="1309" t="s">
         <v>18</v>
       </c>
       <c r="L103" s="111"/>
@@ -20668,8 +20671,8 @@
       <c r="G104" s="112"/>
       <c r="H104" s="50"/>
       <c r="I104" s="50"/>
-      <c r="J104" s="1311"/>
-      <c r="K104" s="1310"/>
+      <c r="J104" s="1306"/>
+      <c r="K104" s="1305"/>
       <c r="L104" s="50"/>
       <c r="M104" s="50"/>
       <c r="N104" s="78"/>
@@ -34950,7 +34953,7 @@
       <c r="P432" s="7"/>
       <c r="R432" s="2"/>
     </row>
-    <row r="433" spans="1:18" ht="409.6">
+    <row r="433" spans="1:18">
       <c r="A433" s="2"/>
       <c r="E433" s="6"/>
       <c r="P433" s="7"/>
@@ -36278,10 +36281,10 @@
   <dimension ref="A1:BG1064"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="W2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AE135" sqref="AE135"/>
+      <selection pane="bottomRight" activeCell="E272" sqref="E272"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" outlineLevelRow="1"/>
@@ -43737,7 +43740,7 @@
       <c r="D131" s="461" t="s">
         <v>2264</v>
       </c>
-      <c r="E131" s="1315" t="s">
+      <c r="E131" s="1310" t="s">
         <v>2268</v>
       </c>
       <c r="F131" s="947" t="s">
@@ -43790,7 +43793,7 @@
       <c r="D132" s="461" t="s">
         <v>1125</v>
       </c>
-      <c r="E132" s="1315" t="s">
+      <c r="E132" s="1310" t="s">
         <v>2266</v>
       </c>
       <c r="F132" s="947" t="s">
@@ -43829,13 +43832,13 @@
       <c r="Y132" s="550" t="s">
         <v>2036</v>
       </c>
-      <c r="Z132" s="1305" t="s">
+      <c r="Z132" s="1312" t="s">
         <v>2044</v>
       </c>
-      <c r="AA132" s="1306"/>
-      <c r="AB132" s="1306"/>
-      <c r="AC132" s="1306"/>
-      <c r="AD132" s="1307"/>
+      <c r="AA132" s="1313"/>
+      <c r="AB132" s="1313"/>
+      <c r="AC132" s="1313"/>
+      <c r="AD132" s="1314"/>
       <c r="AE132" s="862">
         <v>1</v>
       </c>
@@ -43851,7 +43854,7 @@
       <c r="D133" s="461" t="s">
         <v>2265</v>
       </c>
-      <c r="E133" s="1316" t="s">
+      <c r="E133" s="1311" t="s">
         <v>2267</v>
       </c>
       <c r="F133" s="947" t="s">
@@ -43945,13 +43948,13 @@
       <c r="Y134" s="547" t="s">
         <v>2036</v>
       </c>
-      <c r="Z134" s="1305" t="s">
+      <c r="Z134" s="1312" t="s">
         <v>2044</v>
       </c>
-      <c r="AA134" s="1306"/>
-      <c r="AB134" s="1306"/>
-      <c r="AC134" s="1306"/>
-      <c r="AD134" s="1307"/>
+      <c r="AA134" s="1313"/>
+      <c r="AB134" s="1313"/>
+      <c r="AC134" s="1313"/>
+      <c r="AD134" s="1314"/>
       <c r="AE134" s="862"/>
     </row>
     <row r="135" spans="1:31" ht="13.5" collapsed="1" thickBot="1">
@@ -44252,10 +44255,10 @@
       <c r="AB140" s="1289">
         <v>0.1</v>
       </c>
-      <c r="AC140" s="1308" t="s">
+      <c r="AC140" s="1315" t="s">
         <v>2105</v>
       </c>
-      <c r="AD140" s="1309"/>
+      <c r="AD140" s="1316"/>
       <c r="AE140" s="815">
         <v>4</v>
       </c>
@@ -45939,10 +45942,10 @@
       <c r="AB171" s="1289" t="s">
         <v>2260</v>
       </c>
-      <c r="AC171" s="1308" t="s">
+      <c r="AC171" s="1315" t="s">
         <v>2105</v>
       </c>
-      <c r="AD171" s="1309"/>
+      <c r="AD171" s="1316"/>
       <c r="AE171" s="833" t="s">
         <v>2263</v>
       </c>
@@ -46118,10 +46121,10 @@
       <c r="AB174" s="1289" t="s">
         <v>2261</v>
       </c>
-      <c r="AC174" s="1308" t="s">
+      <c r="AC174" s="1315" t="s">
         <v>2105</v>
       </c>
-      <c r="AD174" s="1309"/>
+      <c r="AD174" s="1316"/>
       <c r="AE174" s="833" t="s">
         <v>2263</v>
       </c>
@@ -46237,10 +46240,10 @@
       <c r="AB176" s="1289">
         <v>0.1</v>
       </c>
-      <c r="AC176" s="1308" t="s">
+      <c r="AC176" s="1315" t="s">
         <v>2105</v>
       </c>
-      <c r="AD176" s="1309"/>
+      <c r="AD176" s="1316"/>
       <c r="AE176" s="815">
         <v>4</v>
       </c>
@@ -46308,10 +46311,10 @@
       <c r="AB177" s="1289" t="s">
         <v>2260</v>
       </c>
-      <c r="AC177" s="1308" t="s">
+      <c r="AC177" s="1315" t="s">
         <v>2105</v>
       </c>
-      <c r="AD177" s="1309"/>
+      <c r="AD177" s="1316"/>
       <c r="AE177" s="833" t="s">
         <v>2263</v>
       </c>
@@ -46487,10 +46490,10 @@
       <c r="AB180" s="1289" t="s">
         <v>2261</v>
       </c>
-      <c r="AC180" s="1308" t="s">
+      <c r="AC180" s="1315" t="s">
         <v>2105</v>
       </c>
-      <c r="AD180" s="1309"/>
+      <c r="AD180" s="1316"/>
       <c r="AE180" s="833" t="s">
         <v>2263</v>
       </c>
@@ -46620,10 +46623,10 @@
       <c r="AB182" s="1291">
         <v>0.25</v>
       </c>
-      <c r="AC182" s="1308" t="s">
+      <c r="AC182" s="1315" t="s">
         <v>2105</v>
       </c>
-      <c r="AD182" s="1309"/>
+      <c r="AD182" s="1316"/>
       <c r="AE182" s="833" t="s">
         <v>2263</v>
       </c>
@@ -51928,7 +51931,7 @@
         <v>2008</v>
       </c>
       <c r="E271" s="422" t="s">
-        <v>2017</v>
+        <v>2271</v>
       </c>
       <c r="F271" s="422" t="s">
         <v>1515</v>

</xml_diff>